<commit_message>
Adjusted starting page for application. Updated Scrum paperwork for submission.
</commit_message>
<xml_diff>
--- a/Planning and Design/CST-247-RS-SprintBurnDown - CLC.xlsx
+++ b/Planning and Design/CST-247-RS-SprintBurnDown - CLC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Grand Canyon University\Classes\CST-247\CLC - Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Grand Canyon University\Classes\CST-247\CLC - Week 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18330" windowHeight="9075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
@@ -175,8 +175,8 @@
   </si>
   <si>
     <t>Project Title: Minsweeper Web Application
-Release #: 0.1
-Sprint #: 1</t>
+Release #: 0.2
+Sprint #: 2</t>
   </si>
 </sst>
 </file>
@@ -363,10 +363,96 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Ideal burndown</c:v>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn Down Chart'!$F$14:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5999999999999979</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1999999999999975</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7999999999999976</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3999999999999977</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.2204460492503131E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Actual</c:v>
           </c:tx>
           <c:dLbls>
             <c:spPr>
@@ -386,189 +472,47 @@
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
-                <c15:showLeaderLines val="0"/>
+                <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn Down Chart'!$F$15:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Day 10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 8</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Day 7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Day 6</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Day 5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Day 4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Day 3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$F$19:$O$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Actual burndown</c:v>
-          </c:tx>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Day 10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$F$20:$O$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -586,11 +530,255 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="411988944"/>
-        <c:axId val="411976792"/>
+        <c:axId val="434417496"/>
+        <c:axId val="434418280"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Ideal burndown</c:v>
+                </c:tx>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="0"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$5:$O$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>Day 10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Day 9</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Day 8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Day 7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Day 6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Day 5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Day 4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Day 3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Day 2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Day 1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$19:$O$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>Actual burndown</c:v>
+                </c:tx>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="0"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$5:$O$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>Day 10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Day 9</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Day 8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Day 7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Day 6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Day 5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Day 4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Day 3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Day 2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Day 1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$20:$O$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="411988944"/>
+        <c:axId val="434417496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +788,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="411976792"/>
+        <c:crossAx val="434418280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="411976792"/>
+        <c:axId val="434418280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="411988944"/>
+        <c:crossAx val="434417496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1056,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,10 +1358,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="4">
         <v>0</v>
@@ -1338,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4">
         <v>0</v>
@@ -1469,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -1484,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="4">
         <v>0</v>
@@ -1519,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
@@ -1534,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
@@ -1581,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
@@ -1618,7 +1806,7 @@
         <v>12.6</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" ref="H14:P14" si="0">G14-$F$14/10</f>
+        <f t="shared" ref="H14:O14" si="0">G14-$F$14/10</f>
         <v>11.2</v>
       </c>
       <c r="I14" s="4">
@@ -1650,7 +1838,7 @@
         <v>1.3999999999999977</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" si="0"/>
+        <f>O14-$F$14/10</f>
         <v>-2.2204460492503131E-15</v>
       </c>
       <c r="Q14" s="1"/>
@@ -1670,43 +1858,43 @@
       </c>
       <c r="G15" s="4">
         <f t="shared" ref="G15:P15" si="1">F15 - SUM(G4:G13)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2318,6 +2506,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1251" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c2c36359d71eb747fbb188f75fc8d29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08acee74153637279a480e75df712a71" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2506,25 +2712,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA975265-C41C-4191-AC8E-A5AD70B8A3C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2541,29 +2754,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>